<commit_message>
Auto commit 2025-05-17 17:40:31.88
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\예약\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E450144C-C72A-401F-88B5-55C4AFA4A784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F688A7F2-A639-44E1-9742-174530FB0029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>17:40</t>
+    <t>17:50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Auto commit 2025-05-17 17:57:04.79
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\예약\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F688A7F2-A639-44E1-9742-174530FB0029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93945F3-2A8C-4A63-AC1C-F1B8506562B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,11 +79,11 @@
     <t>15:40</t>
   </si>
   <si>
-    <t>17:00</t>
+    <t>18:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>17:50</t>
+    <t>18:10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Auto commit 2025-05-17 18:31:47.73
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\예약\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93945F3-2A8C-4A63-AC1C-F1B8506562B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0992FB2-46CA-4658-A8E2-9026F14FCDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,11 +79,11 @@
     <t>15:40</t>
   </si>
   <si>
-    <t>18:00</t>
+    <t>6:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>18:10</t>
+    <t>6:40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Auto commit 2025-05-17 18:33:47.51
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\예약\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0992FB2-46CA-4658-A8E2-9026F14FCDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74E0C81-7A34-4598-9D10-F5E57A8B2374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,11 +79,11 @@
     <t>15:40</t>
   </si>
   <si>
-    <t>6:30</t>
+    <t>18:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6:40</t>
+    <t>18:40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Auto commit 2025-05-17 18:41:32.59
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\예약\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74E0C81-7A34-4598-9D10-F5E57A8B2374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A932CE4-585B-4AB6-BFEF-89EFA7EBC4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="17">
   <si>
     <t>교시</t>
   </si>
@@ -77,14 +77,6 @@
   </si>
   <si>
     <t>15:40</t>
-  </si>
-  <si>
-    <t>18:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>18:40</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -903,7 +895,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -920,15 +912,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>

</xml_diff>

<commit_message>
Auto commit 2025-05-19 19:17:59.79
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\예약\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\YKseats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A932CE4-585B-4AB6-BFEF-89EFA7EBC4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D426CA06-1112-4323-BCA3-5994918E193B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="월요일" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -424,9 +425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -505,6 +508,17 @@
       </c>
       <c r="C7" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.30902777777777779</v>
       </c>
     </row>
   </sheetData>
@@ -894,7 +908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Auto commit 2025-05-19 19:22:18.11
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\YKseats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D426CA06-1112-4323-BCA3-5994918E193B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9DA988-00C1-48FA-B3B6-8B02B4C23EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
   <si>
     <t>교시</t>
   </si>
@@ -77,6 +77,14 @@
   </si>
   <si>
     <t>15:40</t>
+  </si>
+  <si>
+    <t>19:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19:25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -119,10 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -514,11 +521,11 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.30555555555555558</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.30902777777777779</v>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit 2025-05-19 19:26:25.85
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\YKseats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9DA988-00C1-48FA-B3B6-8B02B4C23EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E13740-F9EB-4945-9109-DA6750CDA119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>19:25</t>
+    <t>19:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Auto commit 2025-05-19 19:36:43.86
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\YKseats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E13740-F9EB-4945-9109-DA6750CDA119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642E2E2E-32CC-43F1-9C43-D7BEC7A58D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>19:30</t>
+    <t>19:40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Auto commit 2025-05-19 19:45:05.62
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\YKseats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642E2E2E-32CC-43F1-9C43-D7BEC7A58D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B9D093-DCCC-4C95-8EF2-A57F6C17A946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>19:40</t>
+    <t>19:50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Auto commit 2025-05-19 19:50:59.31
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\YKseats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B9D093-DCCC-4C95-8EF2-A57F6C17A946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39E086C-50D9-4F22-922F-2FB41D5D1E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>19:50</t>
+    <t>19:53</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Auto commit 2025-05-19 19:57:46.10
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\YKseats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39E086C-50D9-4F22-922F-2FB41D5D1E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A0A079-7180-4984-8699-9EEF2B3819AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>19:53</t>
+    <t>20:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Auto commit 2025-05-19 20:00:43.04
</commit_message>
<xml_diff>
--- a/data/time.xlsx
+++ b/data/time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sihoo\OneDrive\文档\알고리즘\YKseats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A0A079-7180-4984-8699-9EEF2B3819AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BE0544-4416-48C9-98D4-83239F911DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2745" yWindow="1800" windowWidth="15930" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="17">
   <si>
     <t>교시</t>
   </si>
@@ -77,14 +77,6 @@
   </si>
   <si>
     <t>15:40</t>
-  </si>
-  <si>
-    <t>19:20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -435,7 +427,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -518,15 +510,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>